<commit_message>
partlist and m79 pigtail updates
Reorganized the partlist a lot

Made the M79 to pigtail wirelist more legible for Fred
</commit_message>
<xml_diff>
--- a/pigtail_M79_to_preamp.xlsx
+++ b/pigtail_M79_to_preamp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="99">
   <si>
     <t>Board:</t>
   </si>
@@ -279,69 +279,12 @@
     <t>CRY_ADR_301B</t>
   </si>
   <si>
-    <t>36"</t>
-  </si>
-  <si>
     <t>Phil's wirelist based off Sarah's big document</t>
   </si>
   <si>
     <t>AWG 24</t>
   </si>
   <si>
-    <t>AWG 24, tp #5</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #4</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #41</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #16</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #17</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #42</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #12 &amp; #13</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #15 &amp; #40</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #12 &amp; #39</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #13 &amp; #39</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #14 &amp; #40</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #14 &amp; #15</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #18 &amp; #62</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #18 &amp; #43</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #43 &amp; #62</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #19 &amp; #63</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp # 19 &amp; #44</t>
-  </si>
-  <si>
-    <t>AWG 24, tsp #44 &amp; #63</t>
-  </si>
-  <si>
     <t>M79 circular to D-sub 25 socket</t>
   </si>
   <si>
@@ -354,50 +297,32 @@
     <t>lhe I m</t>
   </si>
   <si>
-    <t>AWG 24, tp #11</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #10</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #37</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #38</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #35</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #36</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #34</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #33</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #7</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #6</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #8</t>
-  </si>
-  <si>
-    <t>AWG 24, tp #9</t>
-  </si>
-  <si>
     <t>Please make cable 4 feet long</t>
+  </si>
+  <si>
+    <t>Twisted With</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>AWG 24, tp</t>
+  </si>
+  <si>
+    <t>AWG 24, tsp</t>
+  </si>
+  <si>
+    <t>48"</t>
+  </si>
+  <si>
+    <t>Reformated so that the pairs/shields are easier to understand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,6 +381,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -754,18 +685,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1137,20 +1057,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O90"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1159,11 +1082,13 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1171,88 +1096,108 @@
         <v>85</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="7">
         <v>41187</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="E5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="7">
+        <v>41204</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="10"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" ht="16" thickBot="1">
+      <c r="E7" s="10"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="16" thickBot="1">
       <c r="A8" s="8"/>
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" ht="16" thickBot="1">
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="16" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
@@ -1260,471 +1205,563 @@
         <v>9</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="F9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="G9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="H9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="2"/>
       <c r="K9" s="9"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="M9" s="9"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="15">
         <v>1</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="15">
+      <c r="F10" s="15">
         <v>6</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="2"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="8"/>
+      <c r="G10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="2"/>
       <c r="K10" s="9"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="M10" s="9"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="18">
+      <c r="F11" s="18">
         <v>7</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="2"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
+      <c r="G11" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="2"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="17">
         <v>3</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="17">
+      <c r="F12" s="17">
         <v>5</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="2"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="G12" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="2"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="17">
         <v>4</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="15">
+        <v>5</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="17">
+      <c r="F13" s="17">
         <v>2</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="2"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="G13" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="2"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="17">
         <v>5</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="15">
+        <v>4</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="17">
+      <c r="F14" s="17">
         <v>4</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="22"/>
-      <c r="G14" s="2"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="G14" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="22"/>
+      <c r="I14" s="2"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="17">
         <v>6</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>109</v>
+      <c r="C15" s="17">
+        <v>33</v>
       </c>
       <c r="D15" s="17"/>
-      <c r="E15" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="2"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="E15" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="23"/>
+      <c r="I15" s="2"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="17">
         <v>7</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>109</v>
+      <c r="C16" s="17">
+        <v>34</v>
       </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="2"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="E16" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="2"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="17">
         <v>8</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>109</v>
+      <c r="C17" s="17">
+        <v>35</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="2"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="E17" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="2"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="17">
         <v>9</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>109</v>
+      <c r="C18" s="17">
+        <v>36</v>
       </c>
       <c r="D18" s="17"/>
-      <c r="E18" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="2"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="E18" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="2"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="17">
         <v>10</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>109</v>
+      <c r="C19" s="17">
+        <v>11</v>
       </c>
       <c r="D19" s="17"/>
-      <c r="E19" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="F19" s="23"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="E19" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="16" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B20" s="17">
         <v>11</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>109</v>
+      <c r="C20" s="17">
+        <v>10</v>
       </c>
       <c r="D20" s="17"/>
-      <c r="E20" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="E20" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="17">
         <v>12</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="15">
+        <v>13</v>
+      </c>
+      <c r="D21" s="15">
+        <v>39</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="17">
+      <c r="F21" s="17">
         <v>17</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="G21" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="17">
         <v>13</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="15">
+        <v>12</v>
+      </c>
+      <c r="D22" s="15">
+        <v>39</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="17">
+      <c r="F22" s="17">
         <v>16</v>
       </c>
-      <c r="E22" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="G22" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="17">
         <v>14</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="15">
+        <v>15</v>
+      </c>
+      <c r="D23" s="15">
+        <v>40</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="17">
+      <c r="F23" s="17">
         <v>24</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="G23" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="H23" s="23"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="17">
         <v>15</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="15">
+        <v>14</v>
+      </c>
+      <c r="D24" s="15">
+        <v>40</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="17">
+      <c r="F24" s="17">
         <v>23</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="G24" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="17">
         <v>16</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="15">
+        <v>41</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="17">
+      <c r="F25" s="17">
         <v>21</v>
       </c>
-      <c r="E25" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="23"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="G25" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" s="23"/>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="17">
         <v>17</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="15">
+        <v>42</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="17">
+      <c r="F26" s="17">
         <v>14</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="G26" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="17">
         <v>18</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="15">
+        <v>43</v>
+      </c>
+      <c r="D27" s="15">
+        <v>62</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="17">
+      <c r="F27" s="17">
         <v>9</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="23"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="G27" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="23"/>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="17">
         <v>19</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="15">
+        <v>44</v>
+      </c>
+      <c r="D28" s="15">
+        <v>63</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="17">
+      <c r="F28" s="17">
         <v>11</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="G28" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="17">
         <v>20</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="17">
+      <c r="F29" s="17">
         <v>19</v>
       </c>
-      <c r="E29" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" s="23"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="G29" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" s="23"/>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="17">
         <v>21</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="17">
+      <c r="F30" s="17">
         <v>20</v>
       </c>
-      <c r="E30" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F30" s="22"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="G30" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="16" t="s">
         <v>30</v>
       </c>
@@ -1733,10 +1770,12 @@
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="23"/>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="23"/>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" s="16" t="s">
         <v>31</v>
       </c>
@@ -1745,10 +1784,12 @@
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="22"/>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="16" t="s">
         <v>32</v>
       </c>
@@ -1757,10 +1798,12 @@
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="23"/>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="23"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="16" t="s">
         <v>33</v>
       </c>
@@ -1769,10 +1812,12 @@
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="22"/>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="16" t="s">
         <v>34</v>
       </c>
@@ -1781,10 +1826,12 @@
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="23"/>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="23"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="16" t="s">
         <v>35</v>
       </c>
@@ -1793,28 +1840,32 @@
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="22"/>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="17">
         <v>28</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="17">
+      <c r="F37" s="17">
         <v>1</v>
       </c>
-      <c r="E37" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F37" s="23"/>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H37" s="23"/>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="16" t="s">
         <v>37</v>
       </c>
@@ -1823,10 +1874,12 @@
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="22"/>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="16" t="s">
         <v>38</v>
       </c>
@@ -1835,10 +1888,12 @@
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="23"/>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="23"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="16" t="s">
         <v>39</v>
       </c>
@@ -1847,232 +1902,284 @@
       </c>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="17">
         <v>32</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="17">
+      <c r="F41" s="17">
         <v>3</v>
       </c>
-      <c r="E41" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F41" s="23"/>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H41" s="23"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="17">
         <v>33</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>109</v>
+      <c r="C42" s="17">
+        <v>6</v>
       </c>
       <c r="D42" s="17"/>
-      <c r="E42" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F42" s="22"/>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="E42" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="G42" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42" s="22"/>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="17">
         <v>34</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>109</v>
+      <c r="C43" s="17">
+        <v>7</v>
       </c>
       <c r="D43" s="17"/>
-      <c r="E43" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F43" s="23"/>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="E43" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="17"/>
+      <c r="G43" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H43" s="23"/>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B44" s="17">
         <v>35</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>109</v>
+      <c r="C44" s="17">
+        <v>8</v>
       </c>
       <c r="D44" s="17"/>
-      <c r="E44" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="E44" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" s="17"/>
+      <c r="G44" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H44" s="22"/>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B45" s="17">
         <v>36</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>109</v>
+      <c r="C45" s="17">
+        <v>9</v>
       </c>
       <c r="D45" s="17"/>
-      <c r="E45" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F45" s="23"/>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="E45" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="G45" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H45" s="23"/>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B46" s="17">
         <v>37</v>
       </c>
-      <c r="C46" s="17" t="s">
-        <v>109</v>
+      <c r="C46" s="17">
+        <v>38</v>
       </c>
       <c r="D46" s="17"/>
-      <c r="E46" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="E46" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="G46" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H46" s="22"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="16" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="B47" s="17">
         <v>38</v>
       </c>
-      <c r="C47" s="20" t="s">
-        <v>109</v>
+      <c r="C47" s="17">
+        <v>37</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F47" s="23"/>
-    </row>
-    <row r="48" spans="1:6">
+        <v>90</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H47" s="23"/>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="17">
         <v>39</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D48" s="17">
+      <c r="F48" s="17">
         <v>18</v>
       </c>
-      <c r="E48" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F48" s="22"/>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H48" s="22"/>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="16" t="s">
         <v>44</v>
       </c>
       <c r="B49" s="17">
         <v>40</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="17">
+      <c r="F49" s="17">
         <v>25</v>
       </c>
-      <c r="E49" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F49" s="23"/>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H49" s="23"/>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B50" s="17">
         <v>41</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="15">
+        <v>16</v>
+      </c>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D50" s="17">
+      <c r="F50" s="17">
         <v>22</v>
       </c>
-      <c r="E50" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F50" s="22"/>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H50" s="22"/>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B51" s="17">
         <v>42</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="15">
+        <v>17</v>
+      </c>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="17">
+      <c r="F51" s="17">
         <v>15</v>
       </c>
-      <c r="E51" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F51" s="23"/>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H51" s="23"/>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B52" s="17">
         <v>43</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="15">
+        <v>18</v>
+      </c>
+      <c r="D52" s="15">
+        <v>63</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D52" s="17">
+      <c r="F52" s="17">
         <v>8</v>
       </c>
-      <c r="E52" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F52" s="22"/>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H52" s="22"/>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B53" s="17">
         <v>44</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="15">
+        <v>19</v>
+      </c>
+      <c r="D53" s="15">
+        <v>63</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D53" s="17">
+      <c r="F53" s="17">
         <v>12</v>
       </c>
-      <c r="E53" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="F53" s="23"/>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H53" s="23"/>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="16" t="s">
         <v>49</v>
       </c>
@@ -2081,10 +2188,12 @@
       </c>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="22"/>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="22"/>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="16" t="s">
         <v>50</v>
       </c>
@@ -2093,10 +2202,12 @@
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="23"/>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="23"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="16" t="s">
         <v>51</v>
       </c>
@@ -2105,10 +2216,12 @@
       </c>
       <c r="C56" s="17"/>
       <c r="D56" s="17"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="22"/>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="22"/>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="16" t="s">
         <v>52</v>
       </c>
@@ -2117,10 +2230,12 @@
       </c>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="23"/>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="23"/>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="16" t="s">
         <v>53</v>
       </c>
@@ -2129,10 +2244,12 @@
       </c>
       <c r="C58" s="17"/>
       <c r="D58" s="17"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="22"/>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="22"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="16" t="s">
         <v>54</v>
       </c>
@@ -2141,10 +2258,12 @@
       </c>
       <c r="C59" s="17"/>
       <c r="D59" s="17"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="23"/>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="23"/>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="16" t="s">
         <v>55</v>
       </c>
@@ -2153,10 +2272,12 @@
       </c>
       <c r="C60" s="17"/>
       <c r="D60" s="17"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="22"/>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="22"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="16" t="s">
         <v>56</v>
       </c>
@@ -2165,10 +2286,12 @@
       </c>
       <c r="C61" s="17"/>
       <c r="D61" s="17"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="23"/>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="23"/>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="16" t="s">
         <v>57</v>
       </c>
@@ -2177,10 +2300,12 @@
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="22"/>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="22"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="16" t="s">
         <v>58</v>
       </c>
@@ -2189,10 +2314,12 @@
       </c>
       <c r="C63" s="17"/>
       <c r="D63" s="17"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="23"/>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="23"/>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="16" t="s">
         <v>59</v>
       </c>
@@ -2201,10 +2328,12 @@
       </c>
       <c r="C64" s="17"/>
       <c r="D64" s="17"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="22"/>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="22"/>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="16" t="s">
         <v>60</v>
       </c>
@@ -2213,10 +2342,12 @@
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="23"/>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="23"/>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="16" t="s">
         <v>61</v>
       </c>
@@ -2225,10 +2356,12 @@
       </c>
       <c r="C66" s="17"/>
       <c r="D66" s="17"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="22"/>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="22"/>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="16" t="s">
         <v>62</v>
       </c>
@@ -2237,10 +2370,12 @@
       </c>
       <c r="C67" s="17"/>
       <c r="D67" s="17"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="23"/>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="23"/>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="16" t="s">
         <v>63</v>
       </c>
@@ -2249,10 +2384,12 @@
       </c>
       <c r="C68" s="17"/>
       <c r="D68" s="17"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="22"/>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="22"/>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="16" t="s">
         <v>64</v>
       </c>
@@ -2261,10 +2398,12 @@
       </c>
       <c r="C69" s="17"/>
       <c r="D69" s="17"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="23"/>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="23"/>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="16" t="s">
         <v>65</v>
       </c>
@@ -2273,46 +2412,52 @@
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="17"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="22"/>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="22"/>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B71" s="17">
         <v>62</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D71" s="17">
+      <c r="F71" s="17">
         <v>10</v>
       </c>
-      <c r="E71" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="F71" s="23"/>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="H71" s="23"/>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="16" t="s">
         <v>67</v>
       </c>
       <c r="B72" s="17">
         <v>63</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D72" s="17">
+      <c r="F72" s="17">
         <v>13</v>
       </c>
-      <c r="E72" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="F72" s="22"/>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H72" s="22"/>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="16" t="s">
         <v>68</v>
       </c>
@@ -2321,10 +2466,12 @@
       </c>
       <c r="C73" s="17"/>
       <c r="D73" s="17"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="23"/>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="23"/>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="16" t="s">
         <v>69</v>
       </c>
@@ -2333,10 +2480,12 @@
       </c>
       <c r="C74" s="17"/>
       <c r="D74" s="17"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="22"/>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="22"/>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="16" t="s">
         <v>70</v>
       </c>
@@ -2345,10 +2494,12 @@
       </c>
       <c r="C75" s="17"/>
       <c r="D75" s="17"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="23"/>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="23"/>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="16" t="s">
         <v>71</v>
       </c>
@@ -2357,10 +2508,12 @@
       </c>
       <c r="C76" s="17"/>
       <c r="D76" s="17"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="22"/>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="22"/>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="16" t="s">
         <v>71</v>
       </c>
@@ -2369,10 +2522,12 @@
       </c>
       <c r="C77" s="17"/>
       <c r="D77" s="17"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="23"/>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="23"/>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="16" t="s">
         <v>72</v>
       </c>
@@ -2381,10 +2536,12 @@
       </c>
       <c r="C78" s="17"/>
       <c r="D78" s="17"/>
-      <c r="E78" s="19"/>
-      <c r="F78" s="22"/>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="22"/>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="16" t="s">
         <v>73</v>
       </c>
@@ -2393,10 +2550,12 @@
       </c>
       <c r="C79" s="17"/>
       <c r="D79" s="17"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="23"/>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="23"/>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="16" t="s">
         <v>74</v>
       </c>
@@ -2405,10 +2564,12 @@
       </c>
       <c r="C80" s="17"/>
       <c r="D80" s="17"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="22"/>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="22"/>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="16" t="s">
         <v>75</v>
       </c>
@@ -2417,10 +2578,12 @@
       </c>
       <c r="C81" s="17"/>
       <c r="D81" s="17"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="23"/>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="E81" s="17"/>
+      <c r="F81" s="17"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="23"/>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="16" t="s">
         <v>76</v>
       </c>
@@ -2429,10 +2592,12 @@
       </c>
       <c r="C82" s="17"/>
       <c r="D82" s="17"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="22"/>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="E82" s="17"/>
+      <c r="F82" s="17"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="22"/>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" s="16" t="s">
         <v>77</v>
       </c>
@@ -2441,10 +2606,12 @@
       </c>
       <c r="C83" s="17"/>
       <c r="D83" s="17"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="23"/>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="23"/>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="16" t="s">
         <v>78</v>
       </c>
@@ -2453,10 +2620,12 @@
       </c>
       <c r="C84" s="17"/>
       <c r="D84" s="17"/>
-      <c r="E84" s="19"/>
-      <c r="F84" s="22"/>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="22"/>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" s="16" t="s">
         <v>79</v>
       </c>
@@ -2465,10 +2634,12 @@
       </c>
       <c r="C85" s="17"/>
       <c r="D85" s="17"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="23"/>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="E85" s="17"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="23"/>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" s="16" t="s">
         <v>80</v>
       </c>
@@ -2477,10 +2648,12 @@
       </c>
       <c r="C86" s="17"/>
       <c r="D86" s="17"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="22"/>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="E86" s="17"/>
+      <c r="F86" s="17"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="22"/>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="16" t="s">
         <v>81</v>
       </c>
@@ -2489,10 +2662,12 @@
       </c>
       <c r="C87" s="17"/>
       <c r="D87" s="17"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="23"/>
-    </row>
-    <row r="88" spans="1:6" ht="16" thickBot="1">
+      <c r="E87" s="17"/>
+      <c r="F87" s="17"/>
+      <c r="G87" s="20"/>
+      <c r="H87" s="23"/>
+    </row>
+    <row r="88" spans="1:8" ht="16" thickBot="1">
       <c r="A88" s="24" t="s">
         <v>82</v>
       </c>
@@ -2501,40 +2676,43 @@
       </c>
       <c r="C88" s="25"/>
       <c r="D88" s="25"/>
-      <c r="E88" s="26"/>
-      <c r="F88" s="27"/>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="26"/>
+      <c r="H88" s="27"/>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="28" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A10:B88 A90">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <phoneticPr fontId="10" type="noConversion"/>
+  <conditionalFormatting sqref="A10:D88 A90">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D88">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="F10:F88">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C88 C10:C45">
-    <cfRule type="expression" dxfId="2" priority="2">
+  <conditionalFormatting sqref="E48:E88 E10:E45">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="E46">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="78" fitToHeight="2" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>